<commit_message>
Added to shed D-sub and tweaked code
Added the pins used for the heater relay to the D-sub pinout document. There has also been lots of work done on the shed non qual code. There is still lots more to go.
</commit_message>
<xml_diff>
--- a/Shed and Weather Station Documents/D-Sub pin-out.xlsx
+++ b/Shed and Weather Station Documents/D-Sub pin-out.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9fbcfc042faff9e2/Projects/Dog Shed and Weather Station/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9fbcfc042faff9e2/Documents/GitHub/shed/Shed and Weather Station Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="257" documentId="8_{78E5F922-F4FE-4E8B-B02A-D9A1D96B03D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41330BD9-F8C2-409A-AEF7-73F0CD1EACE3}"/>
+  <xr:revisionPtr revIDLastSave="261" documentId="8_{78E5F922-F4FE-4E8B-B02A-D9A1D96B03D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9495B3E-1A70-4245-8B74-3032102F2EC2}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C04A02AC-D4FA-4651-B3C6-327C7F5D1E58}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
   <si>
     <t>Pin #</t>
   </si>
@@ -238,13 +238,19 @@
   </si>
   <si>
     <t>this is going to be used for the window switch</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>Thermistor in the relay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,12 +263,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -344,7 +344,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>170497</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>113693</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -699,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF9E575-4207-4084-99BB-88A694C9067F}">
   <dimension ref="A2:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,14 +899,16 @@
       <c r="C16" s="1"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -950,7 +952,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="4"/>
@@ -1026,7 +1028,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="4"/>

</xml_diff>

<commit_message>
Added start_up Loops and window updates
Added startup loops for the light, motor, and heater relays. I also changed the pin to 36 for the window relay and added #define stepsPerRevolution to the shed code.
</commit_message>
<xml_diff>
--- a/Shed and Weather Station Documents/D-Sub pin-out.xlsx
+++ b/Shed and Weather Station Documents/D-Sub pin-out.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9fbcfc042faff9e2/Documents/GitHub/shed/Shed and Weather Station Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="270" documentId="8_{78E5F922-F4FE-4E8B-B02A-D9A1D96B03D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4264170F-35BD-43D7-AEF1-A470A427F100}"/>
+  <xr:revisionPtr revIDLastSave="272" documentId="8_{78E5F922-F4FE-4E8B-B02A-D9A1D96B03D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{991DC489-F714-41E6-BA8D-5A80A662EEDA}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C04A02AC-D4FA-4651-B3C6-327C7F5D1E58}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C04A02AC-D4FA-4651-B3C6-327C7F5D1E58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF9E575-4207-4084-99BB-88A694C9067F}">
   <dimension ref="A2:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>